<commit_message>
Implemented unit tests and started refactoring classes
</commit_message>
<xml_diff>
--- a/QSSD/testing/5 Table merge.xlsx
+++ b/QSSD/testing/5 Table merge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni work\ce301_ramsay_foster_b\QSSD\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\Querying-semi-structured-data\Project\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62BE343-9AA2-462E-B888-F4A490DEEA27}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38D3CBD-329F-48B4-A007-5B111387781A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31065" yWindow="7695" windowWidth="12300" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29235" yWindow="4830" windowWidth="14175" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -232,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,6 +254,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,7 +623,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -637,99 +640,88 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <f ca="1">RANDBETWEEN(2000,3000)</f>
-        <v>2488</v>
+      <c r="B2" s="7">
+        <v>2731</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B12" ca="1" si="0">RANDBETWEEN(2000,3000)</f>
-        <v>2234</v>
+      <c r="B3" s="7">
+        <v>2262</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
-        <f t="shared" ca="1" si="0"/>
-        <v>2231</v>
+      <c r="B4" s="7">
+        <v>2479</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5">
-        <f t="shared" ca="1" si="0"/>
-        <v>2939</v>
+      <c r="B5" s="7">
+        <v>2144</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6">
-        <f t="shared" ca="1" si="0"/>
-        <v>2071</v>
+      <c r="B6" s="7">
+        <v>2845</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7">
-        <f t="shared" ca="1" si="0"/>
-        <v>2022</v>
+      <c r="B7" s="7">
+        <v>2403</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8">
-        <f t="shared" ca="1" si="0"/>
-        <v>2817</v>
+      <c r="B8" s="7">
+        <v>2584</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9">
-        <f t="shared" ca="1" si="0"/>
-        <v>2582</v>
+      <c r="B9" s="7">
+        <v>2147</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10">
-        <f t="shared" ca="1" si="0"/>
-        <v>2994</v>
+      <c r="B10" s="7">
+        <v>2224</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11">
-        <f t="shared" ca="1" si="0"/>
-        <v>2345</v>
+      <c r="B11" s="7">
+        <v>2112</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12">
-        <f t="shared" ca="1" si="0"/>
-        <v>2348</v>
+      <c r="B12" s="7">
+        <v>2149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>